<commit_message>
student competency import excel
</commit_message>
<xml_diff>
--- a/studentCompetency.xlsx
+++ b/studentCompetency.xlsx
@@ -635,7 +635,7 @@
         <v>178</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -655,7 +655,7 @@
         <v>178</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -675,7 +675,7 @@
         <v>178</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -695,7 +695,7 @@
         <v>178</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -715,7 +715,7 @@
         <v>178</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -735,7 +735,7 @@
         <v>178</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -755,7 +755,7 @@
         <v>178</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -775,7 +775,7 @@
         <v>178</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -795,7 +795,7 @@
         <v>178</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -815,7 +815,7 @@
         <v>178</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -835,7 +835,7 @@
         <v>178</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -855,7 +855,7 @@
         <v>178</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -875,7 +875,7 @@
         <v>178</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -895,7 +895,7 @@
         <v>178</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -915,7 +915,7 @@
         <v>178</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -935,7 +935,7 @@
         <v>178</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -955,7 +955,7 @@
         <v>178</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -975,7 +975,7 @@
         <v>178</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -995,7 +995,7 @@
         <v>178</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1015,7 +1015,7 @@
         <v>178</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1035,7 +1035,7 @@
         <v>178</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1055,7 +1055,7 @@
         <v>178</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1075,7 +1075,7 @@
         <v>178</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1095,7 +1095,7 @@
         <v>178</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1115,7 +1115,7 @@
         <v>178</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1135,7 +1135,7 @@
         <v>178</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1155,7 +1155,7 @@
         <v>178</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1175,7 +1175,7 @@
         <v>178</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1226,7 +1226,7 @@
         <v>179</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -1246,7 +1246,7 @@
         <v>179</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1266,7 +1266,7 @@
         <v>179</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1286,7 +1286,7 @@
         <v>179</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1306,7 +1306,7 @@
         <v>179</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1326,7 +1326,7 @@
         <v>179</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1346,7 +1346,7 @@
         <v>179</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1366,7 +1366,7 @@
         <v>179</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1386,7 +1386,7 @@
         <v>179</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1406,7 +1406,7 @@
         <v>179</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1426,7 +1426,7 @@
         <v>179</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1446,7 +1446,7 @@
         <v>179</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1466,7 +1466,7 @@
         <v>179</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -1486,7 +1486,7 @@
         <v>179</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -1506,7 +1506,7 @@
         <v>179</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -1526,7 +1526,7 @@
         <v>179</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -1546,7 +1546,7 @@
         <v>179</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1566,7 +1566,7 @@
         <v>179</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1586,7 +1586,7 @@
         <v>179</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1606,7 +1606,7 @@
         <v>179</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -1626,7 +1626,7 @@
         <v>179</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -1646,7 +1646,7 @@
         <v>179</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -1666,7 +1666,7 @@
         <v>179</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -1686,7 +1686,7 @@
         <v>179</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -1706,7 +1706,7 @@
         <v>179</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -1726,7 +1726,7 @@
         <v>179</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -1746,7 +1746,7 @@
         <v>179</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -1766,7 +1766,7 @@
         <v>179</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -1817,7 +1817,7 @@
         <v>180</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -1837,7 +1837,7 @@
         <v>180</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -1857,7 +1857,7 @@
         <v>180</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -1877,7 +1877,7 @@
         <v>180</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -1897,7 +1897,7 @@
         <v>180</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -1917,7 +1917,7 @@
         <v>180</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -1937,7 +1937,7 @@
         <v>180</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -1957,7 +1957,7 @@
         <v>180</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -1977,7 +1977,7 @@
         <v>180</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -1997,7 +1997,7 @@
         <v>180</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2017,7 +2017,7 @@
         <v>180</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2037,7 +2037,7 @@
         <v>180</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2057,7 +2057,7 @@
         <v>180</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2077,7 +2077,7 @@
         <v>180</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -2097,7 +2097,7 @@
         <v>180</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -2117,7 +2117,7 @@
         <v>180</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -2137,7 +2137,7 @@
         <v>180</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -2157,7 +2157,7 @@
         <v>180</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -2177,7 +2177,7 @@
         <v>180</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -2197,7 +2197,7 @@
         <v>180</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -2217,7 +2217,7 @@
         <v>180</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -2237,7 +2237,7 @@
         <v>180</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -2257,7 +2257,7 @@
         <v>180</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -2277,7 +2277,7 @@
         <v>180</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -2297,7 +2297,7 @@
         <v>180</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -2317,7 +2317,7 @@
         <v>180</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -2337,7 +2337,7 @@
         <v>180</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2357,7 +2357,7 @@
         <v>180</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -2408,7 +2408,7 @@
         <v>181</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2428,7 +2428,7 @@
         <v>181</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -2448,7 +2448,7 @@
         <v>181</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -2468,7 +2468,7 @@
         <v>181</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -2488,7 +2488,7 @@
         <v>181</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -2508,7 +2508,7 @@
         <v>181</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -2528,7 +2528,7 @@
         <v>181</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -2548,7 +2548,7 @@
         <v>181</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -2568,7 +2568,7 @@
         <v>181</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -2588,7 +2588,7 @@
         <v>181</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -2608,7 +2608,7 @@
         <v>181</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -2628,7 +2628,7 @@
         <v>181</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -2648,7 +2648,7 @@
         <v>181</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -2668,7 +2668,7 @@
         <v>181</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -2688,7 +2688,7 @@
         <v>181</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -2708,7 +2708,7 @@
         <v>181</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -2728,7 +2728,7 @@
         <v>181</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>72</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -2748,7 +2748,7 @@
         <v>181</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -2768,7 +2768,7 @@
         <v>181</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -2788,7 +2788,7 @@
         <v>181</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>86</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -2808,7 +2808,7 @@
         <v>181</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -2828,7 +2828,7 @@
         <v>181</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -2848,7 +2848,7 @@
         <v>181</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -2868,7 +2868,7 @@
         <v>181</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>91</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -2888,7 +2888,7 @@
         <v>181</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -2908,7 +2908,7 @@
         <v>181</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="138" spans="1:7">
@@ -2928,7 +2928,7 @@
         <v>181</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="139" spans="1:7">
@@ -2948,7 +2948,7 @@
         <v>181</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="142" spans="1:7">
@@ -2999,7 +2999,7 @@
         <v>182</v>
       </c>
       <c r="F145">
-        <v>0</v>
+        <v>75</v>
       </c>
     </row>
     <row r="146" spans="1:7">
@@ -3019,7 +3019,7 @@
         <v>182</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="147" spans="1:7">
@@ -3039,7 +3039,7 @@
         <v>182</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="148" spans="1:7">
@@ -3059,7 +3059,7 @@
         <v>182</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="149" spans="1:7">
@@ -3079,7 +3079,7 @@
         <v>182</v>
       </c>
       <c r="F149">
-        <v>0</v>
+        <v>63</v>
       </c>
     </row>
     <row r="150" spans="1:7">
@@ -3099,7 +3099,7 @@
         <v>182</v>
       </c>
       <c r="F150">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="151" spans="1:7">
@@ -3119,7 +3119,7 @@
         <v>182</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="152" spans="1:7">
@@ -3139,7 +3139,7 @@
         <v>182</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -3159,7 +3159,7 @@
         <v>182</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -3179,7 +3179,7 @@
         <v>182</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -3199,7 +3199,7 @@
         <v>182</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="156" spans="1:7">
@@ -3219,7 +3219,7 @@
         <v>182</v>
       </c>
       <c r="F156">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="157" spans="1:7">
@@ -3239,7 +3239,7 @@
         <v>182</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="158" spans="1:7">
@@ -3259,7 +3259,7 @@
         <v>182</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="159" spans="1:7">
@@ -3279,7 +3279,7 @@
         <v>182</v>
       </c>
       <c r="F159">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
     <row r="160" spans="1:7">
@@ -3299,7 +3299,7 @@
         <v>182</v>
       </c>
       <c r="F160">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="161" spans="1:7">
@@ -3319,7 +3319,7 @@
         <v>182</v>
       </c>
       <c r="F161">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="162" spans="1:7">
@@ -3339,7 +3339,7 @@
         <v>182</v>
       </c>
       <c r="F162">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="163" spans="1:7">
@@ -3359,7 +3359,7 @@
         <v>182</v>
       </c>
       <c r="F163">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="164" spans="1:7">
@@ -3379,7 +3379,7 @@
         <v>182</v>
       </c>
       <c r="F164">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="165" spans="1:7">
@@ -3399,7 +3399,7 @@
         <v>182</v>
       </c>
       <c r="F165">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="166" spans="1:7">
@@ -3419,7 +3419,7 @@
         <v>182</v>
       </c>
       <c r="F166">
-        <v>0</v>
+        <v>99</v>
       </c>
     </row>
     <row r="167" spans="1:7">
@@ -3439,7 +3439,7 @@
         <v>182</v>
       </c>
       <c r="F167">
-        <v>0</v>
+        <v>95</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -3459,7 +3459,7 @@
         <v>182</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="169" spans="1:7">
@@ -3479,7 +3479,7 @@
         <v>182</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -3499,7 +3499,7 @@
         <v>182</v>
       </c>
       <c r="F170">
-        <v>0</v>
+        <v>74</v>
       </c>
     </row>
     <row r="171" spans="1:7">
@@ -3519,7 +3519,7 @@
         <v>182</v>
       </c>
       <c r="F171">
-        <v>0</v>
+        <v>73</v>
       </c>
     </row>
     <row r="172" spans="1:7">
@@ -3539,7 +3539,7 @@
         <v>182</v>
       </c>
       <c r="F172">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="175" spans="1:7">
@@ -3590,7 +3590,7 @@
         <v>183</v>
       </c>
       <c r="F178">
-        <v>100</v>
+        <v>77</v>
       </c>
     </row>
     <row r="179" spans="1:7">
@@ -3610,7 +3610,7 @@
         <v>183</v>
       </c>
       <c r="F179">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="180" spans="1:7">
@@ -3630,7 +3630,7 @@
         <v>183</v>
       </c>
       <c r="F180">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="181" spans="1:7">
@@ -3650,7 +3650,7 @@
         <v>183</v>
       </c>
       <c r="F181">
-        <v>70</v>
+        <v>97</v>
       </c>
     </row>
     <row r="182" spans="1:7">
@@ -3670,7 +3670,7 @@
         <v>183</v>
       </c>
       <c r="F182">
-        <v>60</v>
+        <v>87</v>
       </c>
     </row>
     <row r="183" spans="1:7">
@@ -3690,7 +3690,7 @@
         <v>183</v>
       </c>
       <c r="F183">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="184" spans="1:7">
@@ -3710,7 +3710,7 @@
         <v>183</v>
       </c>
       <c r="F184">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="185" spans="1:7">
@@ -3730,7 +3730,7 @@
         <v>183</v>
       </c>
       <c r="F185">
-        <v>30</v>
+        <v>78</v>
       </c>
     </row>
     <row r="186" spans="1:7">
@@ -3750,7 +3750,7 @@
         <v>183</v>
       </c>
       <c r="F186">
-        <v>20</v>
+        <v>87</v>
       </c>
     </row>
     <row r="187" spans="1:7">
@@ -3770,7 +3770,7 @@
         <v>183</v>
       </c>
       <c r="F187">
-        <v>10</v>
+        <v>84</v>
       </c>
     </row>
     <row r="188" spans="1:7">
@@ -3790,7 +3790,7 @@
         <v>183</v>
       </c>
       <c r="F188">
-        <v>0</v>
+        <v>97</v>
       </c>
     </row>
     <row r="189" spans="1:7">
@@ -3810,7 +3810,7 @@
         <v>183</v>
       </c>
       <c r="F189">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="190" spans="1:7">
@@ -3830,7 +3830,7 @@
         <v>183</v>
       </c>
       <c r="F190">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="191" spans="1:7">
@@ -3850,7 +3850,7 @@
         <v>183</v>
       </c>
       <c r="F191">
-        <v>0</v>
+        <v>84</v>
       </c>
     </row>
     <row r="192" spans="1:7">
@@ -3870,7 +3870,7 @@
         <v>183</v>
       </c>
       <c r="F192">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="193" spans="1:7">
@@ -3890,7 +3890,7 @@
         <v>183</v>
       </c>
       <c r="F193">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="194" spans="1:7">
@@ -3910,7 +3910,7 @@
         <v>183</v>
       </c>
       <c r="F194">
-        <v>0</v>
+        <v>89</v>
       </c>
     </row>
     <row r="195" spans="1:7">
@@ -3930,7 +3930,7 @@
         <v>183</v>
       </c>
       <c r="F195">
-        <v>0</v>
+        <v>76</v>
       </c>
     </row>
     <row r="196" spans="1:7">
@@ -3950,7 +3950,7 @@
         <v>183</v>
       </c>
       <c r="F196">
-        <v>0</v>
+        <v>70</v>
       </c>
     </row>
     <row r="197" spans="1:7">
@@ -3970,7 +3970,7 @@
         <v>183</v>
       </c>
       <c r="F197">
-        <v>0</v>
+        <v>71</v>
       </c>
     </row>
     <row r="198" spans="1:7">
@@ -3990,7 +3990,7 @@
         <v>183</v>
       </c>
       <c r="F198">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:7">
@@ -4010,7 +4010,7 @@
         <v>183</v>
       </c>
       <c r="F199">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="200" spans="1:7">
@@ -4030,7 +4030,7 @@
         <v>183</v>
       </c>
       <c r="F200">
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="201" spans="1:7">
@@ -4050,7 +4050,7 @@
         <v>183</v>
       </c>
       <c r="F201">
-        <v>0</v>
+        <v>77</v>
       </c>
     </row>
     <row r="202" spans="1:7">
@@ -4070,7 +4070,7 @@
         <v>183</v>
       </c>
       <c r="F202">
-        <v>0</v>
+        <v>57</v>
       </c>
     </row>
     <row r="203" spans="1:7">
@@ -4090,7 +4090,7 @@
         <v>183</v>
       </c>
       <c r="F203">
-        <v>0</v>
+        <v>80</v>
       </c>
     </row>
     <row r="204" spans="1:7">
@@ -4110,7 +4110,7 @@
         <v>183</v>
       </c>
       <c r="F204">
-        <v>0</v>
+        <v>58</v>
       </c>
     </row>
     <row r="205" spans="1:7">
@@ -4130,7 +4130,7 @@
         <v>183</v>
       </c>
       <c r="F205">
-        <v>0</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>